<commit_message>
add auth and fix bugs of table in mail
</commit_message>
<xml_diff>
--- a/uploads/status-by-agent/אושר כהן.xlsx
+++ b/uploads/status-by-agent/אושר כהן.xlsx
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -397,565 +398,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>שם פרטי</v>
+        <v>סוג תהליך</v>
       </c>
       <c r="B1" t="str">
-        <v>שם משפחה</v>
+        <v>סטטוס</v>
       </c>
       <c r="C1" t="str">
-        <v>סטטוס</v>
+        <v>תאריך יצירה</v>
       </c>
       <c r="D1" t="str">
+        <v>שם מטפל</v>
+      </c>
+      <c r="E1" t="str">
+        <v>לקוח</v>
+      </c>
+      <c r="F1" t="str">
         <v>שם סוכן</v>
       </c>
-      <c r="E1" t="str">
-        <v>שם מטפל</v>
-      </c>
-      <c r="F1" t="str">
-        <v>הערות</v>
-      </c>
       <c r="G1" t="str">
-        <v>תאריך יצירה</v>
-      </c>
-      <c r="H1" t="str">
-        <v>תאריך שינוי</v>
-      </c>
-      <c r="I1" t="str">
-        <v>תחום</v>
+        <v>סוג מוצר חדש</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>יבגניה*</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B2" t="str">
-        <v>פונומריוב</v>
+        <v>לא מעוניין</v>
       </c>
       <c r="C2" t="str">
-        <v>הצעה</v>
+        <v>01.05.2023</v>
       </c>
       <c r="D2" t="str">
-        <v>אושר כהן</v>
+        <v>חני עדס</v>
       </c>
       <c r="E2" t="str">
-        <v xml:space="preserve">בר כוכבא ריקי </v>
+        <v>ניסים תומר</v>
       </c>
       <c r="F2" t="str">
-        <v xml:space="preserve">בוצע גבייה 6.11.23ככ דג מ כדגמכדגלךכ מדגךלכ דגךכלמ חצד גכדג ככדגשגשדג שדגשדגשד גשדג שדג שדגשדג דשג שדג שדג  שגדשדגשדגשדג שדג שדג שד גשד </v>
+        <v>אושר כהן</v>
       </c>
       <c r="G2" t="str">
-        <v>15.01.2023</v>
-      </c>
-      <c r="H2" t="str">
-        <v>16.05.2024</v>
-      </c>
-      <c r="I2" t="str">
-        <v>החזרי מס</v>
+        <v>ביטוח חיים משכנתא</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>מיגיר</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B3" t="str">
-        <v>לוייב</v>
+        <v>דרושה פגישת המשך</v>
       </c>
       <c r="C3" t="str">
-        <v xml:space="preserve">הצעה </v>
+        <v>28.05.2023</v>
       </c>
       <c r="D3" t="str">
-        <v>אושר כהן</v>
+        <v>מלכה מסבנד</v>
       </c>
       <c r="E3" t="str">
-        <v>לוי הודיה</v>
+        <v>זוסמן תומר</v>
       </c>
       <c r="F3" t="str">
-        <v>בוצע חישוב לא זכאי להחזר</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G3" t="str">
-        <v>30.03.2023</v>
-      </c>
-      <c r="H3" t="str">
-        <v>12.02.2024</v>
-      </c>
-      <c r="I3" t="str">
-        <v>החזרי מס</v>
+        <v>-</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>אושרת מסעודה</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B4" t="str">
-        <v>עודני</v>
+        <v>נשלח להפקה</v>
       </c>
       <c r="C4" t="str">
-        <v>הופק</v>
+        <v>24.05.2023</v>
       </c>
       <c r="D4" t="str">
-        <v>אושר כהן</v>
+        <v>מלכה מסבנד</v>
       </c>
       <c r="E4" t="str">
-        <v>יהוד ספיר</v>
+        <v>לוין אורנה</v>
       </c>
       <c r="F4" t="str">
-        <v>בוצע גבייה 11.04.24</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G4" t="str">
-        <v>03.07.2023</v>
-      </c>
-      <c r="H4" t="str">
-        <v>15.04.2024</v>
-      </c>
-      <c r="I4" t="str">
-        <v>החזרי מס</v>
+        <v>ביטוח חיים משכנתא</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>מישל וורד</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B5" t="str">
-        <v>שוקרני</v>
+        <v>בתהליך החתמת טפסים</v>
       </c>
       <c r="C5" t="str">
-        <v xml:space="preserve">שאלון </v>
+        <v>24.05.2023</v>
       </c>
       <c r="D5" t="str">
-        <v>אושר כהן</v>
+        <v>יוכבד פרץ</v>
       </c>
       <c r="E5" t="str">
-        <v xml:space="preserve">כלפון טל </v>
+        <v>מלכה דוד</v>
       </c>
       <c r="F5" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G5" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H5" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I5" t="str">
-        <v>החזרי מס</v>
+        <v>ביטוח חיים משכנתא</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>יבגניה*</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B6" t="str">
-        <v>פונומריוב</v>
+        <v>בתהליך החתמת טפסים</v>
       </c>
       <c r="C6" t="str">
-        <v>הצעה</v>
+        <v>24.05.2023</v>
       </c>
       <c r="D6" t="str">
-        <v>אושר כהן</v>
+        <v>יוכבד פרץ</v>
       </c>
       <c r="E6" t="str">
-        <v xml:space="preserve">בר כוכבא ריקי </v>
+        <v>מלכה מיכל</v>
       </c>
       <c r="F6" t="str">
-        <v>בוצע גבייה 6.11.23</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G6" t="str">
-        <v>15.01.2023</v>
-      </c>
-      <c r="H6" t="str">
-        <v>16.05.2024</v>
-      </c>
-      <c r="I6" t="str">
-        <v>החזרי מס</v>
+        <v>ביטוח חיים משכנתא</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>מיגיר</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B7" t="str">
-        <v>לוייב</v>
+        <v>דרושה פגישת המשך</v>
       </c>
       <c r="C7" t="str">
-        <v xml:space="preserve">הצעה </v>
+        <v>21.05.2023</v>
       </c>
       <c r="D7" t="str">
-        <v>אושר כהן</v>
+        <v>חני עדס</v>
       </c>
       <c r="E7" t="str">
-        <v>לוי הודיה</v>
+        <v>חנון אהרון יאיר</v>
       </c>
       <c r="F7" t="str">
-        <v>בוצע חישוב לא זכאי להחזר</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G7" t="str">
-        <v>30.03.2023</v>
-      </c>
-      <c r="H7" t="str">
-        <v>12.02.2024</v>
-      </c>
-      <c r="I7" t="str">
-        <v>החזרי מס</v>
+        <v>-</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>אושרת מסעודה</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B8" t="str">
-        <v>עודני</v>
+        <v>דרושה פגישת המשך</v>
       </c>
       <c r="C8" t="str">
-        <v>הופק</v>
+        <v>21.05.2023</v>
       </c>
       <c r="D8" t="str">
-        <v>אושר כהן</v>
+        <v>מלכה מסבנד</v>
       </c>
       <c r="E8" t="str">
-        <v>יהוד ספיר</v>
+        <v>מימרן רפאל</v>
       </c>
       <c r="F8" t="str">
-        <v>בוצע גבייה 11.04.24</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G8" t="str">
-        <v>03.07.2023</v>
-      </c>
-      <c r="H8" t="str">
-        <v>15.04.2024</v>
-      </c>
-      <c r="I8" t="str">
-        <v>החזרי מס</v>
+        <v>-</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>מישל וורד</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B9" t="str">
-        <v>שוקרני</v>
+        <v>דרושה פגישת המשך</v>
       </c>
       <c r="C9" t="str">
-        <v xml:space="preserve">שאלון </v>
+        <v>21.05.2023</v>
       </c>
       <c r="D9" t="str">
-        <v>אושר כהן</v>
+        <v>מלכה מסבנד</v>
       </c>
       <c r="E9" t="str">
-        <v xml:space="preserve">כלפון טל </v>
+        <v>הופמן אהרון</v>
       </c>
       <c r="F9" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G9" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H9" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I9" t="str">
-        <v>החזרי מס</v>
+        <v>-</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>מישל וורד</v>
+        <v>הצטרפות בריאות וריסק</v>
       </c>
       <c r="B10" t="str">
-        <v>שוקרני</v>
+        <v>דרושה פגישת המשך</v>
       </c>
       <c r="C10" t="str">
-        <v xml:space="preserve">שאלון </v>
+        <v>21.05.2023</v>
       </c>
       <c r="D10" t="str">
-        <v>אושר כהן</v>
+        <v>מלכה מסבנד</v>
       </c>
       <c r="E10" t="str">
-        <v xml:space="preserve">כלפון טל </v>
+        <v>ירסקי ליאת</v>
       </c>
       <c r="F10" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
+        <v>אושר כהן</v>
       </c>
       <c r="G10" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H10" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I10" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>יבגניה*</v>
-      </c>
-      <c r="B11" t="str">
-        <v>פונומריוב</v>
-      </c>
-      <c r="C11" t="str">
-        <v>הצעה</v>
-      </c>
-      <c r="D11" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E11" t="str">
-        <v xml:space="preserve">בר כוכבא ריקי </v>
-      </c>
-      <c r="F11" t="str">
-        <v>בוצע גבייה 6.11.23</v>
-      </c>
-      <c r="G11" t="str">
-        <v>15.01.2023</v>
-      </c>
-      <c r="H11" t="str">
-        <v>16.05.2024</v>
-      </c>
-      <c r="I11" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>מיגיר</v>
-      </c>
-      <c r="B12" t="str">
-        <v>לוייב</v>
-      </c>
-      <c r="C12" t="str">
-        <v xml:space="preserve">הצעה </v>
-      </c>
-      <c r="D12" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E12" t="str">
-        <v>לוי הודיה</v>
-      </c>
-      <c r="F12" t="str">
-        <v>בוצע חישוב לא זכאי להחזר</v>
-      </c>
-      <c r="G12" t="str">
-        <v>30.03.2023</v>
-      </c>
-      <c r="H12" t="str">
-        <v>12.02.2024</v>
-      </c>
-      <c r="I12" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>אושרת מסעודה</v>
-      </c>
-      <c r="B13" t="str">
-        <v>עודני</v>
-      </c>
-      <c r="C13" t="str">
-        <v>הופק</v>
-      </c>
-      <c r="D13" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E13" t="str">
-        <v>יהוד ספיר</v>
-      </c>
-      <c r="F13" t="str">
-        <v>בוצע גבייה 11.04.24</v>
-      </c>
-      <c r="G13" t="str">
-        <v>03.07.2023</v>
-      </c>
-      <c r="H13" t="str">
-        <v>15.04.2024</v>
-      </c>
-      <c r="I13" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>מישל וורד</v>
-      </c>
-      <c r="B14" t="str">
-        <v>שוקרני</v>
-      </c>
-      <c r="C14" t="str">
-        <v xml:space="preserve">שאלון </v>
-      </c>
-      <c r="D14" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E14" t="str">
-        <v xml:space="preserve">כלפון טל </v>
-      </c>
-      <c r="F14" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
-      </c>
-      <c r="G14" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H14" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I14" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>מישל וורד</v>
-      </c>
-      <c r="B15" t="str">
-        <v>שוקרני</v>
-      </c>
-      <c r="C15" t="str">
-        <v xml:space="preserve">שאלון </v>
-      </c>
-      <c r="D15" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E15" t="str">
-        <v xml:space="preserve">כלפון טל </v>
-      </c>
-      <c r="F15" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
-      </c>
-      <c r="G15" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H15" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I15" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>יבגניה*</v>
-      </c>
-      <c r="B16" t="str">
-        <v>פונומריוב</v>
-      </c>
-      <c r="C16" t="str">
-        <v>הצעה</v>
-      </c>
-      <c r="D16" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E16" t="str">
-        <v xml:space="preserve">בר כוכבא ריקי </v>
-      </c>
-      <c r="F16" t="str">
-        <v>בוצע גבייה 6.11.23</v>
-      </c>
-      <c r="G16" t="str">
-        <v>15.01.2023</v>
-      </c>
-      <c r="H16" t="str">
-        <v>16.05.2024</v>
-      </c>
-      <c r="I16" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>מיגיר</v>
-      </c>
-      <c r="B17" t="str">
-        <v>לוייב</v>
-      </c>
-      <c r="C17" t="str">
-        <v xml:space="preserve">הצעה </v>
-      </c>
-      <c r="D17" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E17" t="str">
-        <v>לוי הודיה</v>
-      </c>
-      <c r="F17" t="str">
-        <v>בוצע חישוב לא זכאי להחזר</v>
-      </c>
-      <c r="G17" t="str">
-        <v>30.03.2023</v>
-      </c>
-      <c r="H17" t="str">
-        <v>12.02.2024</v>
-      </c>
-      <c r="I17" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>אושרת מסעודה</v>
-      </c>
-      <c r="B18" t="str">
-        <v>עודני</v>
-      </c>
-      <c r="C18" t="str">
-        <v>הופק</v>
-      </c>
-      <c r="D18" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E18" t="str">
-        <v>יהוד ספיר</v>
-      </c>
-      <c r="F18" t="str">
-        <v>בוצע גבייה 11.04.24</v>
-      </c>
-      <c r="G18" t="str">
-        <v>03.07.2023</v>
-      </c>
-      <c r="H18" t="str">
-        <v>15.04.2024</v>
-      </c>
-      <c r="I18" t="str">
-        <v>החזרי מס</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>מישל וורד</v>
-      </c>
-      <c r="B19" t="str">
-        <v>שוקרני</v>
-      </c>
-      <c r="C19" t="str">
-        <v xml:space="preserve">שאלון </v>
-      </c>
-      <c r="D19" t="str">
-        <v>אושר כהן</v>
-      </c>
-      <c r="E19" t="str">
-        <v xml:space="preserve">כלפון טל </v>
-      </c>
-      <c r="F19" t="str">
-        <v>הוגש למס הכנסה 26.03.24</v>
-      </c>
-      <c r="G19" t="str">
-        <v>12.12.2023</v>
-      </c>
-      <c r="H19" t="str">
-        <v>26.03.2024</v>
-      </c>
-      <c r="I19" t="str">
-        <v>החזרי מס</v>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>